<commit_message>
added standardization algo, added stimuli_info, updated IK code to correctly work with the arm
</commit_message>
<xml_diff>
--- a/Being Creative Research Project/data/stimuli_info_sheet.xlsx
+++ b/Being Creative Research Project/data/stimuli_info_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2ed100b9df88b388/Documents/GitHub/Being-Creative-Research-Project/Being Creative Research Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4554158B-2DE5-49AE-AFEB-B1E4FDEAE1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="8_{4554158B-2DE5-49AE-AFEB-B1E4FDEAE1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E18E64D-66D2-4487-B5C3-6D9A6CF17AEC}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{76824D07-45A9-4273-B76D-5C3E570B60D1}"/>
+    <workbookView xWindow="12257" yWindow="0" windowWidth="12514" windowHeight="14794" xr2:uid="{76824D07-45A9-4273-B76D-5C3E570B60D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Stimuli List" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>category</t>
   </si>
@@ -129,6 +129,13 @@
   </si>
   <si>
     <t xml:space="preserve">A minimalist line art illustration "resting mind" reflecting calmness and contemplation. The design captures stillness and introspection, symbolizing moments of pause and mental clarity. try to be creative and somewhat abstract. </t>
+  </si>
+  <si>
+    <t>A minimalist line illustration of a bottle with a glass nested inside, creating a simple yet clever composition. This artwork captures the beauty of modern minimalism, perfect for those who appreciate refined, abstract line art.
+how creative and abstract can you be? focus on it being inside</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This minimalist line art illustration features a geometric interpretation of a dog, blending simplicity and precision. Created with clean lines and abstract shapes, it highlights the beauty of symmetry and modern design. Perfect for pet lovers, contemporary art collections, and decor enthusiasts, this artwork embodies elegance and creativity while celebrating canine charm. </t>
   </si>
 </sst>
 </file>
@@ -505,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3EE3B82-0408-4307-96CF-0675ACEAC59B}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -557,7 +564,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" ht="131.15" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
@@ -568,7 +575,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="87.45" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" ht="262.3" x14ac:dyDescent="0.4">
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
@@ -579,7 +586,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" ht="131.15" x14ac:dyDescent="0.4">
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
@@ -590,15 +597,18 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" ht="204" x14ac:dyDescent="0.4">
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
+      <c r="D7" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="174.9" x14ac:dyDescent="0.4">
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
@@ -609,12 +619,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="102" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" ht="247.75" x14ac:dyDescent="0.4">
       <c r="B9" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C9" t="s">
         <v>20</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="87.45" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
updated data and analysis
</commit_message>
<xml_diff>
--- a/Being Creative Research Project/data/stimuli_info_sheet.xlsx
+++ b/Being Creative Research Project/data/stimuli_info_sheet.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2ed100b9df88b388/Documents/GitHub/Being-Creative-Research-Project/Being Creative Research Project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{4554158B-2DE5-49AE-AFEB-B1E4FDEAE1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FC19EF7-5F10-4F15-AEF3-8BFEEF3D5C97}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="8_{4554158B-2DE5-49AE-AFEB-B1E4FDEAE1CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BD91CE9-0FBF-4BD7-BC1F-6687F60C5FF8}"/>
   <bookViews>
-    <workbookView xWindow="12257" yWindow="0" windowWidth="12514" windowHeight="14794" xr2:uid="{76824D07-45A9-4273-B76D-5C3E570B60D1}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" activeTab="2" xr2:uid="{76824D07-45A9-4273-B76D-5C3E570B60D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Stimuli List" sheetId="1" r:id="rId1"/>
+    <sheet name="stroke_complexity" sheetId="2" r:id="rId2"/>
+    <sheet name="statistical analysis" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="74">
   <si>
     <t>category</t>
   </si>
@@ -142,13 +145,130 @@
   </si>
   <si>
     <t>A minimalist line art illustration Composed of geometric forms and delicate curves, the figure captures the essence of classical ballet — discipline, strength, and elegance born from tradition.  evoke the timeless poise of ballet schools. how creative and abstract could you be</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>Stroke Count</t>
+  </si>
+  <si>
+    <t>on_the_peak</t>
+  </si>
+  <si>
+    <t>on_the_peak_AI</t>
+  </si>
+  <si>
+    <t>take_it_slow</t>
+  </si>
+  <si>
+    <t>take_it_slow_AI</t>
+  </si>
+  <si>
+    <t>coffee_mind</t>
+  </si>
+  <si>
+    <t>coffee_mind_AI</t>
+  </si>
+  <si>
+    <t>geometric_dog</t>
+  </si>
+  <si>
+    <t>geometric_dog_AI</t>
+  </si>
+  <si>
+    <t>lost_in_a_page</t>
+  </si>
+  <si>
+    <t>lost_in_a_page_AI</t>
+  </si>
+  <si>
+    <t>bottle_and_glass</t>
+  </si>
+  <si>
+    <t>bottle_and_glass_AI</t>
+  </si>
+  <si>
+    <t>resting_mind</t>
+  </si>
+  <si>
+    <t>resting_mind_AI</t>
+  </si>
+  <si>
+    <t>rolled_into_a_paper_roll</t>
+  </si>
+  <si>
+    <t>rolled_into_a_paper_roll_AI</t>
+  </si>
+  <si>
+    <t>russian_ballerina</t>
+  </si>
+  <si>
+    <t>russian_ballerina_AI</t>
+  </si>
+  <si>
+    <t>the_readers_touch</t>
+  </si>
+  <si>
+    <t>the_readers_touch_AI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set B </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Set A </t>
+  </si>
+  <si>
+    <t>mean rating</t>
+  </si>
+  <si>
+    <t>standard deviation</t>
+  </si>
+  <si>
+    <t>Unlabeled Human</t>
+  </si>
+  <si>
+    <t>Unlabeled AI</t>
+  </si>
+  <si>
+    <t>Labeled Human</t>
+  </si>
+  <si>
+    <t>Labeled AI</t>
+  </si>
+  <si>
+    <t>number of ratings</t>
+  </si>
+  <si>
+    <t>Unlabeled Human vs AI</t>
+  </si>
+  <si>
+    <t>Labeled AI vs Unlabeled AI</t>
+  </si>
+  <si>
+    <t>Unlabeled Human vs Labeled Human</t>
+  </si>
+  <si>
+    <t>p - value</t>
+  </si>
+  <si>
+    <t>t - stat</t>
+  </si>
+  <si>
+    <t>significant</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,13 +276,46 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF231F20"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF231F20"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -177,11 +330,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -197,6 +364,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -518,8 +689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3EE3B82-0408-4307-96CF-0675ACEAC59B}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="B11" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -559,7 +730,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="58.3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:5" ht="102" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
@@ -662,4 +833,380 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{928B9BA7-0074-4762-8820-88B0C77ECB0B}">
+  <dimension ref="A1:B28"/>
+  <sheetViews>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="22.921875" customWidth="1"/>
+    <col min="2" max="2" width="23.84375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A11" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A13" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A14" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A15" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15" s="4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A16" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A17" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A18" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="4">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A19" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="4">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A20" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A21" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A23" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A24" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A25" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A26" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A27" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A28" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{937EF260-0FCB-4E61-B3FA-A641856B82AD}">
+  <dimension ref="A1:L6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="3.84375" style="6" customWidth="1"/>
+    <col min="2" max="2" width="19.61328125" customWidth="1"/>
+    <col min="3" max="3" width="17.07421875" customWidth="1"/>
+    <col min="4" max="4" width="11.69140625" customWidth="1"/>
+    <col min="5" max="5" width="17.765625" customWidth="1"/>
+    <col min="6" max="6" width="18.921875" customWidth="1"/>
+    <col min="7" max="7" width="3.23046875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="12.61328125" customWidth="1"/>
+    <col min="9" max="9" width="19.61328125" customWidth="1"/>
+    <col min="10" max="10" width="22.4609375" customWidth="1"/>
+    <col min="11" max="11" width="31.61328125" customWidth="1"/>
+    <col min="12" max="12" width="3.3828125" style="6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="K2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3">
+        <v>134</v>
+      </c>
+      <c r="D3">
+        <v>135</v>
+      </c>
+      <c r="E3">
+        <v>134</v>
+      </c>
+      <c r="F3">
+        <v>133</v>
+      </c>
+      <c r="H3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="7">
+        <v>-4.0490000000000004</v>
+      </c>
+      <c r="J3" s="7">
+        <v>2.7050000000000001</v>
+      </c>
+      <c r="K3">
+        <v>0.317</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4">
+        <v>3.8</v>
+      </c>
+      <c r="D4">
+        <v>4.5</v>
+      </c>
+      <c r="E4">
+        <v>3.75</v>
+      </c>
+      <c r="F4">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="H4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" s="7">
+        <v>1E-4</v>
+      </c>
+      <c r="J4" s="7">
+        <v>7.3000000000000001E-3</v>
+      </c>
+      <c r="K4">
+        <v>0.75170000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.4">
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5">
+        <v>1.39</v>
+      </c>
+      <c r="D5">
+        <v>1.44</v>
+      </c>
+      <c r="E5">
+        <v>1.31</v>
+      </c>
+      <c r="F5">
+        <v>1.43</v>
+      </c>
+      <c r="H5" t="s">
+        <v>71</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="K5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.4"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>